<commit_message>
fixed issues with loading data from models
</commit_message>
<xml_diff>
--- a/src/evaluation/rectools_top5_comparison_results.xlsx
+++ b/src/evaluation/rectools_top5_comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,46 +503,86 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>mmr</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1949358868961792</v>
+        <v>0.7134361190331808</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1799999999999999</v>
+        <v>0.5110410933649582</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.03778289221327196</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7925925925925925</v>
+        <v>0.1931026812795729</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.00909090909090909</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2169312169312169</v>
+        <v>0.005726110502104429</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2619047619047619</v>
+        <v>0.005227462901366726</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4818177150966346</v>
+        <v>0.008377837609220288</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2169312169312169</v>
+        <v>0.00231934626038035</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0.01796536796536797</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2169312169312169</v>
+        <v>0.003506940450404207</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.03778289221327196</v>
       </c>
       <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0.03011123897199847</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.180425360411634</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.03011123897199847</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ready for data from deep learning
</commit_message>
<xml_diff>
--- a/src/evaluation/rectools_top5_comparison_results.xlsx
+++ b/src/evaluation/rectools_top5_comparison_results.xlsx
@@ -503,84 +503,84 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>mmr</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.7134361190331808</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.5110410933649582</v>
-      </c>
+          <t>mf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>0.03778289221327196</v>
+        <v>0.03011123897199847</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1931026812795729</v>
+        <v>0.180425360411634</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00909090909090909</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.005726110502104429</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.005227462901366726</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.008377837609220288</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00231934626038035</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01796536796536797</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003506940450404207</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.03778289221327196</v>
+        <v>0.03011123897199847</v>
       </c>
       <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>mf</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+          <t>mmr</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7134361190331808</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.5110410933649582</v>
+      </c>
       <c r="D3" t="n">
-        <v>0.03011123897199847</v>
+        <v>0.03778289221327196</v>
       </c>
       <c r="E3" t="n">
-        <v>0.180425360411634</v>
+        <v>0.1931026812795729</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.00909090909090909</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.005726110502104429</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.005227462901366726</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.008377837609220288</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.00231934626038035</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.01796536796536797</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>0.003506940450404207</v>
       </c>
       <c r="M3" t="n">
-        <v>0.03011123897199847</v>
+        <v>0.03778289221327196</v>
       </c>
       <c r="N3" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Added So NN data will work with it.
</commit_message>
<xml_diff>
--- a/src/evaluation/rectools_top5_comparison_results.xlsx
+++ b/src/evaluation/rectools_top5_comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,86 +503,46 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>mf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.431730128664218</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.527280469920079</v>
+      </c>
       <c r="D2" t="n">
-        <v>0.03011123897199847</v>
+        <v>0.06518861681005957</v>
       </c>
       <c r="E2" t="n">
-        <v>0.180425360411634</v>
+        <v>0.2813446562071336</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.9013412816691506</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.1679717659980404</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.2482472170010725</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.9046274984948548</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.1592793133421149</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.9526080476900149</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.6016746531844853</v>
       </c>
       <c r="M2" t="n">
-        <v>0.03011123897199847</v>
+        <v>0.06518861681005957</v>
       </c>
       <c r="N2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>mmr</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.7134361190331808</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.5110410933649582</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.03778289221327196</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.1931026812795729</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.00909090909090909</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.005726110502104429</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.005227462901366726</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.008377837609220288</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.00231934626038035</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.01796536796536797</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.003506940450404207</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.03778289221327196</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed it so it should now work, ild i still maybee troublesome
</commit_message>
<xml_diff>
--- a/src/evaluation/rectools_top5_comparison_results.xlsx
+++ b/src/evaluation/rectools_top5_comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,46 +503,130 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>mf</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1.032138758722124</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.7652540722461235</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01731744981248621</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.180425360411634</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.04113263785394933</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.003100835403920611</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.005311706154370903</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.04087925014736316</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.001466035986383272</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.08211624441132637</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.00192577578732003</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.01731744981248621</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>mmr</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.009170831239415</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.7302371529881306</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.02172953893668652</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1931026812795729</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.02175856929955291</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.00129118620221949</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.002334409549589788</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.02036073997695226</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0005748124404458528</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.03899652260307997</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.0007728069700867142</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.02172953893668652</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
           <t>NN</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>4.431730128664218</v>
-      </c>
-      <c r="C2" t="n">
-        <v>3.527280469920079</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
         <v>0.06518861681005957</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E4" t="n">
         <v>0.2813446562071336</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F4" t="n">
         <v>0.9013412816691506</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G4" t="n">
         <v>0.1679717659980404</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H4" t="n">
         <v>0.2482472170010725</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I4" t="n">
         <v>0.9046274984948548</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J4" t="n">
         <v>0.1592793133421149</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K4" t="n">
         <v>0.9526080476900149</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L4" t="n">
         <v>0.6016746531844853</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M4" t="n">
         <v>0.06518861681005957</v>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added hit rate to metrics
</commit_message>
<xml_diff>
--- a/src/evaluation/rectools_top5_comparison_results.xlsx
+++ b/src/evaluation/rectools_top5_comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,45 +456,50 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>HitRate@5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Precision@5</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Recall@5</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>F1@5</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>NDCG@5</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>MAP@5</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>MRR@5</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>PartialAUC@5</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Coverage@5</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>ILD@5</t>
         </is>
@@ -519,30 +524,33 @@
         <v>0.180425360411634</v>
       </c>
       <c r="F2" t="n">
+        <v>0.165424739195231</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.04113263785394933</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.003100835403920611</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.005311706154370903</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.04087925014736316</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.001466035986383272</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.08211624441132637</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.00192577578732003</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.01731744981248621</v>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -563,30 +571,33 @@
         <v>0.1931026812795729</v>
       </c>
       <c r="F3" t="n">
+        <v>0.09239940387481371</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.02175856929955291</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.00129118620221949</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.002334409549589788</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.02036073997695226</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.0005748124404458528</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.03899652260307997</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.0007728069700867142</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.02172953893668652</v>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -603,30 +614,33 @@
         <v>0.2813446562071336</v>
       </c>
       <c r="F4" t="n">
+        <v>0.9985096870342772</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.9013412816691506</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>0.1679717659980404</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>0.2482472170010725</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>0.9046274984948548</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.1592793133421149</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.9526080476900149</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.6016746531844853</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>0.06518861681005957</v>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>